<commit_message>
Aligns carbon tax projections with BNEF base 2H 2024 scenario
</commit_message>
<xml_diff>
--- a/InputData/fuels/FoICStCT/Fraction of Industry Category Subject to Carbon Tax.xlsx
+++ b/InputData/fuels/FoICStCT/Fraction of Industry Category Subject to Carbon Tax.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\fuels\FoICStCT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\fuels\FoICStCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0082FC7F-E8EB-499C-9B98-CAB6A9F10B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F18C19-349B-42A1-B3FD-5C126DFCF6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="636" activeTab="4" xr2:uid="{9AA6BDF2-7B91-4567-88A2-0D83F9E3E450}"/>
+    <workbookView xWindow="35835" yWindow="3240" windowWidth="19185" windowHeight="11265" tabRatio="636" firstSheet="2" activeTab="6" xr2:uid="{9AA6BDF2-7B91-4567-88A2-0D83F9E3E450}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="134">
   <si>
     <t>Unit: dimensionless</t>
   </si>
@@ -456,9 +456,6 @@
     <t>Bloomberg New Energy Finance (BNEF)</t>
   </si>
   <si>
-    <t>EU ETS Market Outlook 1H 2024</t>
-  </si>
-  <si>
     <t>Proprietary report - data on "ETS Projections" page</t>
   </si>
   <si>
@@ -472,6 +469,15 @@
   </si>
   <si>
     <t>Additional Carbon Tax (Elec)</t>
+  </si>
+  <si>
+    <t>old^</t>
+  </si>
+  <si>
+    <t>new^</t>
+  </si>
+  <si>
+    <t>EU ETS Market Outlook 2H 2024</t>
   </si>
 </sst>
 </file>
@@ -1847,94 +1853,94 @@
             <c:numRef>
               <c:f>'ETS Projections'!$C$30:$AE$30</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>86.084369999999993</c:v>
+                  <c:v>86.339434799999992</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>85</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>65</c:v>
+                <c:pt idx="2">
+                  <c:v>63.789062500000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76.48183556405354</c:v>
+                  <c:v>67.724665391969438</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>87.242026266416502</c:v>
+                  <c:v>80.262664165103189</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>95.764272559852671</c:v>
+                  <c:v>95.727440147329659</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100.36166365280289</c:v>
+                  <c:v>102.31464737793851</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>112.78863232682059</c:v>
+                  <c:v>115.20426287744226</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>127.39965095986037</c:v>
+                  <c:v>126.84118673647468</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>137.22126929674101</c:v>
+                  <c:v>133.36052658215647</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>141.65261382799326</c:v>
+                  <c:v>134.58767739188337</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>146.76616915422886</c:v>
+                  <c:v>134.56255154707881</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>151.71288743882545</c:v>
+                  <c:v>138.80097879282221</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>155.69823434991974</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>161.12056091931996</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>166.28468146160586</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>171.44880200389176</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>176.61292254617766</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>181.77704308846356</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>186.94116363074943</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>192.10528417303533</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>197.26940471532123</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>202.43352525760713</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>207.85585182700731</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>213.01997236929321</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>218.18409291157911</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>223.34821345386501</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>228.51233399615089</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>233.67645453843679</c:v>
+                  <c:v>141.7063222183987</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0">
+                  <c:v>146.64136826580562</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0">
+                  <c:v>151.34141212047891</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0">
+                  <c:v>156.04145597515216</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0">
+                  <c:v>160.74149982982544</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0">
+                  <c:v>165.44154368449873</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0">
+                  <c:v>170.14158753917195</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="0">
+                  <c:v>174.84163139384518</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0">
+                  <c:v>179.54167524851843</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0">
+                  <c:v>184.24171910319166</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="0">
+                  <c:v>189.17676515059858</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="0">
+                  <c:v>193.87680900527187</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="0">
+                  <c:v>198.57685285994512</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="0">
+                  <c:v>203.27689671461837</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0">
+                  <c:v>207.97694056929163</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="0">
+                  <c:v>212.67698442396488</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3576,16 +3582,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>5417</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>131109</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>601325</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>553327</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>150159</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3615,8 +3621,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3781425" y="5476875"/>
-          <a:ext cx="4774769" cy="2914650"/>
+          <a:off x="610535" y="5902138"/>
+          <a:ext cx="4738910" cy="2887756"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3637,16 +3643,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>196850</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>172570</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>379319</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>138951</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>526676</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>48559</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>702795</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>11766</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3669,6 +3675,113 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2049" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA400B0D-3C30-346E-F764-8A284173603E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="6464300"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600262</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>32514</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>8033</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DD10C03-4E9A-3D12-EF72-305063F5EC29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="9929" t="51045" r="7749" b="2162"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5396380" y="5803543"/>
+          <a:ext cx="5271620" cy="3023519"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4173,8 +4286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE5FEEC-01CE-4291-999E-35B30A1256CF}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4350,13 +4463,13 @@
     <row r="27" spans="1:7">
       <c r="A27" s="1"/>
       <c r="B27" s="10" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="1"/>
       <c r="B28" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -4469,7 +4582,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4737,7 +4850,7 @@
   <dimension ref="B1:AG11"/>
   <sheetViews>
     <sheetView zoomScale="72" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5704,8 +5817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A6696F-E709-439B-8FAB-66782F7350DF}">
   <dimension ref="A1:AE70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62"/>
+    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6912,46 +7025,46 @@
         <v>118</v>
       </c>
       <c r="C28">
-        <v>81</v>
+        <v>81.239999999999995</v>
       </c>
       <c r="D28">
         <v>85</v>
       </c>
       <c r="E28">
-        <v>65</v>
+        <v>65.320000000000007</v>
       </c>
       <c r="F28">
-        <v>80</v>
+        <v>70.840000000000032</v>
       </c>
       <c r="G28">
-        <v>93</v>
+        <v>85.56</v>
       </c>
       <c r="H28">
-        <v>104</v>
+        <v>103.96000000000001</v>
       </c>
       <c r="I28">
-        <v>111</v>
+        <v>113.16000000000001</v>
       </c>
       <c r="J28">
-        <v>127</v>
+        <v>129.72</v>
       </c>
       <c r="K28">
-        <v>146</v>
+        <v>145.36000000000001</v>
       </c>
       <c r="L28">
-        <v>160</v>
+        <v>155.49837399479443</v>
       </c>
       <c r="M28">
-        <v>168</v>
+        <v>159.62098538677367</v>
       </c>
       <c r="N28">
-        <v>177</v>
+        <v>162.28243716577705</v>
       </c>
       <c r="O28">
-        <v>186</v>
+        <v>170.17000000000002</v>
       </c>
       <c r="P28">
-        <v>194</v>
+        <v>176.56607748412478</v>
       </c>
       <c r="Q28" s="39"/>
       <c r="R28" s="39"/>
@@ -6981,8 +7094,9 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="E29">
-        <v>65</v>
+      <c r="E29" s="3">
+        <f>1/(1+SUM(I4))</f>
+        <v>0.9765625</v>
       </c>
       <c r="F29" s="3">
         <f>1/(1+SUM(I4:I5))</f>
@@ -7046,131 +7160,132 @@
     </row>
     <row r="30" spans="1:31">
       <c r="B30" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" s="39">
+        <v>128</v>
+      </c>
+      <c r="C30" s="19">
         <f>C28*C29</f>
-        <v>86.084369999999993</v>
-      </c>
-      <c r="D30" s="39">
+        <v>86.339434799999992</v>
+      </c>
+      <c r="D30" s="19">
         <f t="shared" ref="D30:P30" si="2">D28*D29</f>
         <v>85</v>
       </c>
-      <c r="E30">
-        <v>65</v>
-      </c>
-      <c r="F30" s="39">
+      <c r="E30" s="19">
+        <f>E28*E29</f>
+        <v>63.789062500000007</v>
+      </c>
+      <c r="F30" s="19">
+        <f>F28*F29</f>
+        <v>67.724665391969438</v>
+      </c>
+      <c r="G30" s="19">
         <f t="shared" si="2"/>
-        <v>76.48183556405354</v>
-      </c>
-      <c r="G30" s="39">
+        <v>80.262664165103189</v>
+      </c>
+      <c r="H30" s="19">
         <f t="shared" si="2"/>
-        <v>87.242026266416502</v>
-      </c>
-      <c r="H30" s="39">
+        <v>95.727440147329659</v>
+      </c>
+      <c r="I30" s="19">
         <f t="shared" si="2"/>
-        <v>95.764272559852671</v>
-      </c>
-      <c r="I30" s="39">
+        <v>102.31464737793851</v>
+      </c>
+      <c r="J30" s="19">
         <f t="shared" si="2"/>
-        <v>100.36166365280289</v>
-      </c>
-      <c r="J30" s="39">
+        <v>115.20426287744226</v>
+      </c>
+      <c r="K30" s="19">
         <f t="shared" si="2"/>
-        <v>112.78863232682059</v>
-      </c>
-      <c r="K30" s="39">
+        <v>126.84118673647468</v>
+      </c>
+      <c r="L30" s="19">
         <f t="shared" si="2"/>
-        <v>127.39965095986037</v>
-      </c>
-      <c r="L30" s="39">
+        <v>133.36052658215647</v>
+      </c>
+      <c r="M30" s="19">
         <f t="shared" si="2"/>
-        <v>137.22126929674101</v>
-      </c>
-      <c r="M30" s="39">
+        <v>134.58767739188337</v>
+      </c>
+      <c r="N30" s="19">
         <f t="shared" si="2"/>
-        <v>141.65261382799326</v>
-      </c>
-      <c r="N30" s="39">
+        <v>134.56255154707881</v>
+      </c>
+      <c r="O30" s="19">
         <f t="shared" si="2"/>
-        <v>146.76616915422886</v>
-      </c>
-      <c r="O30" s="39">
+        <v>138.80097879282221</v>
+      </c>
+      <c r="P30" s="19">
         <f t="shared" si="2"/>
-        <v>151.71288743882545</v>
-      </c>
-      <c r="P30" s="39">
-        <f t="shared" si="2"/>
-        <v>155.69823434991974</v>
+        <v>141.7063222183987</v>
       </c>
       <c r="Q30" s="39">
         <f>Q31/$S3</f>
-        <v>161.12056091931996</v>
+        <v>146.64136826580562</v>
       </c>
       <c r="R30" s="39">
         <f t="shared" ref="R30:AE30" si="3">R31/$S3</f>
-        <v>166.28468146160586</v>
+        <v>151.34141212047891</v>
       </c>
       <c r="S30" s="39">
         <f t="shared" si="3"/>
-        <v>171.44880200389176</v>
+        <v>156.04145597515216</v>
       </c>
       <c r="T30" s="39">
         <f t="shared" si="3"/>
-        <v>176.61292254617766</v>
+        <v>160.74149982982544</v>
       </c>
       <c r="U30" s="39">
         <f t="shared" si="3"/>
-        <v>181.77704308846356</v>
+        <v>165.44154368449873</v>
       </c>
       <c r="V30" s="39">
         <f t="shared" si="3"/>
-        <v>186.94116363074943</v>
+        <v>170.14158753917195</v>
       </c>
       <c r="W30" s="39">
         <f t="shared" si="3"/>
-        <v>192.10528417303533</v>
+        <v>174.84163139384518</v>
       </c>
       <c r="X30" s="39">
         <f t="shared" si="3"/>
-        <v>197.26940471532123</v>
+        <v>179.54167524851843</v>
       </c>
       <c r="Y30" s="39">
         <f t="shared" si="3"/>
-        <v>202.43352525760713</v>
+        <v>184.24171910319166</v>
       </c>
       <c r="Z30" s="39">
         <f t="shared" si="3"/>
-        <v>207.85585182700731</v>
+        <v>189.17676515059858</v>
       </c>
       <c r="AA30" s="39">
         <f t="shared" si="3"/>
-        <v>213.01997236929321</v>
+        <v>193.87680900527187</v>
       </c>
       <c r="AB30" s="39">
         <f t="shared" si="3"/>
-        <v>218.18409291157911</v>
+        <v>198.57685285994512</v>
       </c>
       <c r="AC30" s="39">
         <f t="shared" si="3"/>
-        <v>223.34821345386501</v>
+        <v>203.27689671461837</v>
       </c>
       <c r="AD30" s="39">
         <f t="shared" si="3"/>
-        <v>228.51233399615089</v>
+        <v>207.97694056929163</v>
       </c>
       <c r="AE30" s="39">
         <f t="shared" si="3"/>
-        <v>233.67645453843679</v>
+        <v>212.67698442396488</v>
       </c>
     </row>
     <row r="31" spans="1:31">
       <c r="B31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C31" s="39">
         <f>C30*$S3</f>
-        <v>70.256002454352</v>
+        <v>70.464168387550075</v>
       </c>
       <c r="D31" s="39">
         <f t="shared" ref="D31:P31" si="4">D30*$S3</f>
@@ -7178,111 +7293,119 @@
       </c>
       <c r="E31" s="39">
         <f t="shared" si="4"/>
-        <v>53.048423999999997</v>
+        <v>52.060142062500006</v>
       </c>
       <c r="F31" s="39">
         <f t="shared" si="4"/>
-        <v>62.419089866156789</v>
+        <v>55.27210407648186</v>
       </c>
       <c r="G31" s="39">
         <f t="shared" si="4"/>
-        <v>71.200800000000001</v>
+        <v>65.504735999999994</v>
       </c>
       <c r="H31" s="39">
         <f t="shared" si="4"/>
-        <v>78.156057458563538</v>
+        <v>78.125997436464104</v>
       </c>
       <c r="I31" s="39">
         <f t="shared" si="4"/>
-        <v>81.908124412296559</v>
+        <v>83.502012238698015</v>
       </c>
       <c r="J31" s="39">
         <f t="shared" si="4"/>
-        <v>92.050141385435154</v>
+        <v>94.021608980461806</v>
       </c>
       <c r="K31" s="39">
         <f t="shared" si="4"/>
-        <v>103.97462617801045</v>
+        <v>103.51884699476439</v>
       </c>
       <c r="L31" s="39">
         <f t="shared" si="4"/>
-        <v>111.99033962264153</v>
+        <v>108.83947321528473</v>
       </c>
       <c r="M31" s="39">
         <f t="shared" si="4"/>
-        <v>115.60689106239461</v>
+        <v>109.84098731476682</v>
       </c>
       <c r="N31" s="39">
         <f t="shared" si="4"/>
-        <v>119.78021492537314</v>
+        <v>109.82048136909681</v>
       </c>
       <c r="O31" s="39">
         <f t="shared" si="4"/>
-        <v>123.81737814029364</v>
+        <v>113.27958730179448</v>
       </c>
       <c r="P31" s="39">
         <f t="shared" si="4"/>
-        <v>127.06993772070626</v>
+        <v>115.65072406957285</v>
       </c>
       <c r="Q31" s="39">
         <f>P31*Q13/P13</f>
-        <v>131.49525893486023</v>
+        <v>119.67836122622464</v>
       </c>
       <c r="R31" s="39">
         <f t="shared" ref="R31:AE31" si="5">Q31*R13/Q13</f>
-        <v>135.7098505673878</v>
+        <v>123.51420613732159</v>
       </c>
       <c r="S31" s="39">
         <f t="shared" si="5"/>
-        <v>139.92444219991538</v>
+        <v>127.35005104841855</v>
       </c>
       <c r="T31" s="39">
         <f t="shared" si="5"/>
-        <v>144.13903383244295</v>
+        <v>131.18589595951551</v>
       </c>
       <c r="U31" s="39">
         <f t="shared" si="5"/>
-        <v>148.35362546497052</v>
+        <v>135.02174087061246</v>
       </c>
       <c r="V31" s="39">
         <f t="shared" si="5"/>
-        <v>152.56821709749809</v>
+        <v>138.85758578170939</v>
       </c>
       <c r="W31" s="39">
         <f t="shared" si="5"/>
-        <v>156.78280873002566</v>
+        <v>142.69343069280632</v>
       </c>
       <c r="X31" s="39">
         <f t="shared" si="5"/>
-        <v>160.99740036255324</v>
+        <v>146.52927560390324</v>
       </c>
       <c r="Y31" s="39">
         <f t="shared" si="5"/>
-        <v>165.21199199508081</v>
+        <v>150.36512051500017</v>
       </c>
       <c r="Z31" s="39">
         <f t="shared" si="5"/>
-        <v>169.63731320923475</v>
+        <v>154.39275767165196</v>
       </c>
       <c r="AA31" s="39">
         <f t="shared" si="5"/>
-        <v>173.85190484176232</v>
+        <v>158.22860258274892</v>
       </c>
       <c r="AB31" s="39">
         <f t="shared" si="5"/>
-        <v>178.06649647428989</v>
+        <v>162.06444749384588</v>
       </c>
       <c r="AC31" s="39">
         <f t="shared" si="5"/>
-        <v>182.28108810681746</v>
+        <v>165.9002924049428</v>
       </c>
       <c r="AD31" s="39">
         <f t="shared" si="5"/>
-        <v>186.49567973934504</v>
+        <v>169.73613731603976</v>
       </c>
       <c r="AE31" s="39">
         <f t="shared" si="5"/>
-        <v>190.71027137187261</v>
+        <v>173.57198222713669</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31">
+      <c r="B50" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:31" s="6" customFormat="1">
@@ -7989,7 +8112,7 @@
       </c>
       <c r="C64" s="41">
         <f t="shared" ref="C64:AE64" si="12">MAX(C57,C30)</f>
-        <v>86.084369999999993</v>
+        <v>86.339434799999992</v>
       </c>
       <c r="D64" s="41">
         <f t="shared" si="12"/>
@@ -7997,35 +8120,35 @@
       </c>
       <c r="E64" s="41">
         <f t="shared" si="12"/>
-        <v>65</v>
+        <v>63.789062500000007</v>
       </c>
       <c r="F64" s="41">
         <f t="shared" si="12"/>
-        <v>76.48183556405354</v>
+        <v>67.724665391969438</v>
       </c>
       <c r="G64" s="41">
         <f t="shared" si="12"/>
-        <v>87.242026266416502</v>
+        <v>80.262664165103189</v>
       </c>
       <c r="H64" s="41">
-        <f t="shared" si="12"/>
-        <v>95.764272559852671</v>
+        <f>MAX(H57,H30)</f>
+        <v>95.727440147329659</v>
       </c>
       <c r="I64" s="41">
         <f t="shared" si="12"/>
-        <v>100.36166365280289</v>
+        <v>102.31464737793851</v>
       </c>
       <c r="J64" s="41">
         <f t="shared" si="12"/>
-        <v>112.78863232682059</v>
+        <v>115.20426287744226</v>
       </c>
       <c r="K64" s="41">
         <f t="shared" si="12"/>
-        <v>127.39965095986037</v>
+        <v>126.84118673647468</v>
       </c>
       <c r="L64" s="41">
         <f t="shared" si="12"/>
-        <v>137.22126929674101</v>
+        <v>133.36052658215647</v>
       </c>
       <c r="M64" s="41">
         <f t="shared" si="12"/>
@@ -8150,79 +8273,79 @@
       </c>
       <c r="M65">
         <f t="shared" si="13"/>
-        <v>0.96735992063863285</v>
+        <v>0.91911276045243906</v>
       </c>
       <c r="N65">
         <f t="shared" si="13"/>
-        <v>0.89453570621505807</v>
+        <v>0.82015499738072961</v>
       </c>
       <c r="O65">
         <f t="shared" si="13"/>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="P65">
         <f t="shared" si="13"/>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="Q65" s="41">
         <f t="shared" si="13"/>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="R65">
         <f t="shared" si="13"/>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="S65">
         <f t="shared" si="13"/>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="T65">
         <f t="shared" si="13"/>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="U65">
         <f t="shared" si="13"/>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="V65">
         <f t="shared" si="13"/>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="W65">
         <f t="shared" si="13"/>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="X65">
         <f t="shared" si="13"/>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="Y65">
         <f t="shared" si="13"/>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="Z65">
         <f t="shared" si="13"/>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AA65">
         <f t="shared" si="13"/>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AB65">
         <f t="shared" si="13"/>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AC65">
         <f t="shared" si="13"/>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AD65">
         <f t="shared" si="13"/>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AE65">
         <f t="shared" si="13"/>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="66" spans="2:31">
@@ -8241,8 +8364,8 @@
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="F66">
-        <f t="shared" si="14"/>
+      <c r="F66" s="41">
+        <f>F57/F64</f>
         <v>0</v>
       </c>
       <c r="G66">
@@ -8250,24 +8373,24 @@
         <v>0</v>
       </c>
       <c r="H66">
-        <f t="shared" si="14"/>
-        <v>0.48235390993499733</v>
+        <f>H57/H64</f>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I66">
         <f t="shared" si="14"/>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J66">
         <f t="shared" si="14"/>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K66">
         <f t="shared" si="14"/>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L66">
         <f t="shared" si="14"/>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M66">
         <f t="shared" si="14"/>
@@ -8348,11 +8471,11 @@
     </row>
     <row r="68" spans="2:31">
       <c r="B68" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C68" s="31">
         <f>C64-C63</f>
-        <v>42.953965221151144</v>
+        <v>43.209030021151143</v>
       </c>
       <c r="D68" s="31">
         <f t="shared" ref="D68:AE68" si="15">D64-D63</f>
@@ -8360,35 +8483,35 @@
       </c>
       <c r="E68" s="31">
         <f t="shared" si="15"/>
-        <v>21.869595221151151</v>
+        <v>20.658657721151158</v>
       </c>
       <c r="F68" s="31">
         <f t="shared" si="15"/>
-        <v>33.351430785204691</v>
+        <v>24.594260613120589</v>
       </c>
       <c r="G68" s="31">
-        <f t="shared" si="15"/>
-        <v>40.435734716643033</v>
+        <f>G64-G63</f>
+        <v>33.45637261532972</v>
       </c>
       <c r="H68" s="31">
         <f t="shared" si="15"/>
-        <v>45.282094239154581</v>
+        <v>45.24526182663157</v>
       </c>
       <c r="I68" s="31">
         <f t="shared" si="15"/>
-        <v>46.08106900214937</v>
+        <v>48.034052727284994</v>
       </c>
       <c r="J68" s="31">
         <f t="shared" si="15"/>
-        <v>54.83215090524245</v>
+        <v>57.247781455864121</v>
       </c>
       <c r="K68" s="31">
         <f t="shared" si="15"/>
-        <v>65.767282767357614</v>
+        <v>65.20881854397193</v>
       </c>
       <c r="L68" s="31">
         <f t="shared" si="15"/>
-        <v>73.138309923621847</v>
+        <v>69.277567209037301</v>
       </c>
       <c r="M68" s="31">
         <f t="shared" si="15"/>
@@ -8469,63 +8592,63 @@
     </row>
     <row r="69" spans="2:31">
       <c r="B69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C69">
         <f>C31/MAX($C31:$AE31)</f>
-        <v>0.36839128773173085</v>
+        <v>0.40596510729099416</v>
       </c>
       <c r="D69">
-        <f t="shared" ref="D69:AE69" si="16">D31/MAX($C31:$AE31)</f>
-        <v>0.36375081164208001</v>
+        <f>D31/MAX($C31:$AE31)</f>
+        <v>0.39966713008566629</v>
       </c>
       <c r="E69">
-        <f t="shared" si="16"/>
-        <v>0.2781623853733553</v>
+        <f t="shared" ref="E69:AE69" si="16">E31/MAX($C31:$AE31)</f>
+        <v>0.29993401812035531</v>
       </c>
       <c r="F69">
         <f t="shared" si="16"/>
-        <v>0.3272979972035362</v>
+        <v>0.3184390900378879</v>
       </c>
       <c r="G69">
         <f t="shared" si="16"/>
-        <v>0.37334538663186673</v>
+        <v>0.37739233693995816</v>
       </c>
       <c r="H69">
         <f t="shared" si="16"/>
-        <v>0.40981566905835037</v>
+        <v>0.45010719146036049</v>
       </c>
       <c r="I69">
         <f t="shared" si="16"/>
-        <v>0.42948984248772343</v>
+        <v>0.48108001745020745</v>
       </c>
       <c r="J69">
         <f t="shared" si="16"/>
-        <v>0.4826700770927192</v>
+        <v>0.54168655432778845</v>
       </c>
       <c r="K69">
         <f t="shared" si="16"/>
-        <v>0.54519678164196361</v>
+        <v>0.59640297740737558</v>
       </c>
       <c r="L69">
         <f t="shared" si="16"/>
-        <v>0.58722762448524679</v>
+        <v>0.62705669324474933</v>
       </c>
       <c r="M69">
         <f t="shared" si="16"/>
-        <v>0.6061912147194668</v>
+        <v>0.63282671491893583</v>
       </c>
       <c r="N69">
         <f t="shared" si="16"/>
-        <v>0.6280742723699948</v>
+        <v>0.63270857404500624</v>
       </c>
       <c r="O69">
         <f t="shared" si="16"/>
-        <v>0.64924336402866223</v>
+        <v>0.65263751584951402</v>
       </c>
       <c r="P69">
         <f t="shared" si="16"/>
-        <v>0.66629834254143638</v>
+        <v>0.66629834254143649</v>
       </c>
       <c r="Q69">
         <f t="shared" si="16"/>
@@ -8537,23 +8660,23 @@
       </c>
       <c r="S69">
         <f t="shared" si="16"/>
-        <v>0.73370165745856353</v>
+        <v>0.73370165745856375</v>
       </c>
       <c r="T69">
         <f t="shared" si="16"/>
-        <v>0.75580110497237574</v>
+        <v>0.75580110497237596</v>
       </c>
       <c r="U69">
         <f t="shared" si="16"/>
-        <v>0.77790055248618784</v>
+        <v>0.77790055248618817</v>
       </c>
       <c r="V69">
         <f t="shared" si="16"/>
-        <v>0.8</v>
+        <v>0.80000000000000027</v>
       </c>
       <c r="W69">
         <f t="shared" si="16"/>
-        <v>0.82209944751381214</v>
+        <v>0.82209944751381225</v>
       </c>
       <c r="X69">
         <f t="shared" si="16"/>
@@ -8573,7 +8696,7 @@
       </c>
       <c r="AB69">
         <f t="shared" si="16"/>
-        <v>0.93370165745856348</v>
+        <v>0.93370165745856359</v>
       </c>
       <c r="AC69">
         <f t="shared" si="16"/>
@@ -8581,7 +8704,7 @@
       </c>
       <c r="AD69">
         <f t="shared" si="16"/>
-        <v>0.97790055248618779</v>
+        <v>0.9779005524861879</v>
       </c>
       <c r="AE69">
         <f t="shared" si="16"/>
@@ -8591,7 +8714,7 @@
     <row r="70" spans="2:31">
       <c r="C70" t="str">
         <f>"("&amp;C62&amp;","&amp;ROUND(C68/MAX($C68:$AE68),3)&amp;"),"</f>
-        <v>(2022,0.223),</v>
+        <v>(2022,0.225),</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" ref="D70:AE70" si="17">"("&amp;D62&amp;","&amp;ROUND(D68/MAX($C68:$AE68),3)&amp;"),"</f>
@@ -8599,15 +8722,15 @@
       </c>
       <c r="E70" t="str">
         <f t="shared" si="17"/>
-        <v>(2024,0.114),</v>
+        <v>(2024,0.107),</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="17"/>
-        <v>(2025,0.173),</v>
+        <v>(2025,0.128),</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="17"/>
-        <v>(2026,0.21),</v>
+        <v>(2026,0.174),</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="17"/>
@@ -8615,19 +8738,19 @@
       </c>
       <c r="I70" t="str">
         <f t="shared" si="17"/>
-        <v>(2028,0.239),</v>
+        <v>(2028,0.25),</v>
       </c>
       <c r="J70" t="str">
         <f t="shared" si="17"/>
-        <v>(2029,0.285),</v>
+        <v>(2029,0.297),</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" si="17"/>
-        <v>(2030,0.342),</v>
+        <v>(2030,0.339),</v>
       </c>
       <c r="L70" t="str">
         <f t="shared" si="17"/>
-        <v>(2031,0.38),</v>
+        <v>(2031,0.36),</v>
       </c>
       <c r="M70" t="str">
         <f t="shared" si="17"/>
@@ -8722,7 +8845,7 @@
   <dimension ref="A1:AG28"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8989,23 +9112,23 @@
       </c>
       <c r="J5" s="8">
         <f>IF('ETS Coverage'!$B9=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B5)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B5)),IF('ETS Coverage'!$B9=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K5" s="8">
         <f>IF('ETS Coverage'!$B9=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B5)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B5)),IF('ETS Coverage'!$B9=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L5" s="8">
         <f>IF('ETS Coverage'!$B9=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B5)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B5)),IF('ETS Coverage'!$B9=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M5" s="8">
         <f>IF('ETS Coverage'!$B9=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B5)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B5)),IF('ETS Coverage'!$B9=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N5" s="8">
         <f>IF('ETS Coverage'!$B9=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B5)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B5)),IF('ETS Coverage'!$B9=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O5" s="8">
         <f>IF('ETS Coverage'!$B9=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B5)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B5)),IF('ETS Coverage'!$B9=2,'ETS Projections'!M$66,0))</f>
@@ -9116,23 +9239,23 @@
       </c>
       <c r="J6" s="8">
         <f>IF('ETS Coverage'!$B10=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B6)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B6)),IF('ETS Coverage'!$B10=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K6" s="8">
         <f>IF('ETS Coverage'!$B10=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B6)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B6)),IF('ETS Coverage'!$B10=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L6" s="8">
         <f>IF('ETS Coverage'!$B10=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B6)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B6)),IF('ETS Coverage'!$B10=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M6" s="8">
         <f>IF('ETS Coverage'!$B10=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B6)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B6)),IF('ETS Coverage'!$B10=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N6" s="8">
         <f>IF('ETS Coverage'!$B10=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B6)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B6)),IF('ETS Coverage'!$B10=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O6" s="8">
         <f>IF('ETS Coverage'!$B10=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B6)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B6)),IF('ETS Coverage'!$B10=2,'ETS Projections'!M$66,0))</f>
@@ -9243,23 +9366,23 @@
       </c>
       <c r="J7" s="8">
         <f>IF('ETS Coverage'!$B11=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B7)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B7)),IF('ETS Coverage'!$B11=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K7" s="8">
         <f>IF('ETS Coverage'!$B11=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B7)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B7)),IF('ETS Coverage'!$B11=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L7" s="8">
         <f>IF('ETS Coverage'!$B11=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B7)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B7)),IF('ETS Coverage'!$B11=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M7" s="8">
         <f>IF('ETS Coverage'!$B11=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B7)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B7)),IF('ETS Coverage'!$B11=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N7" s="8">
         <f>IF('ETS Coverage'!$B11=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B7)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B7)),IF('ETS Coverage'!$B11=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O7" s="8">
         <f>IF('ETS Coverage'!$B11=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B7)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B7)),IF('ETS Coverage'!$B11=2,'ETS Projections'!M$66,0))</f>
@@ -9370,23 +9493,23 @@
       </c>
       <c r="J8" s="8">
         <f>IF('ETS Coverage'!$B12=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B8)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B8)),IF('ETS Coverage'!$B12=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K8" s="8">
         <f>IF('ETS Coverage'!$B12=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B8)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B8)),IF('ETS Coverage'!$B12=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L8" s="8">
         <f>IF('ETS Coverage'!$B12=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B8)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B8)),IF('ETS Coverage'!$B12=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M8" s="8">
         <f>IF('ETS Coverage'!$B12=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B8)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B8)),IF('ETS Coverage'!$B12=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N8" s="8">
         <f>IF('ETS Coverage'!$B12=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B8)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B8)),IF('ETS Coverage'!$B12=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O8" s="8">
         <f>IF('ETS Coverage'!$B12=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B8)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B8)),IF('ETS Coverage'!$B12=2,'ETS Projections'!M$66,0))</f>
@@ -9497,23 +9620,23 @@
       </c>
       <c r="J9" s="8">
         <f>IF('ETS Coverage'!$B13=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B9)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B9)),IF('ETS Coverage'!$B13=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K9" s="8">
         <f>IF('ETS Coverage'!$B13=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B9)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B9)),IF('ETS Coverage'!$B13=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L9" s="8">
         <f>IF('ETS Coverage'!$B13=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B9)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B9)),IF('ETS Coverage'!$B13=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M9" s="8">
         <f>IF('ETS Coverage'!$B13=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B9)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B9)),IF('ETS Coverage'!$B13=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N9" s="8">
         <f>IF('ETS Coverage'!$B13=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B9)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B9)),IF('ETS Coverage'!$B13=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O9" s="8">
         <f>IF('ETS Coverage'!$B13=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B9)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B9)),IF('ETS Coverage'!$B13=2,'ETS Projections'!M$66,0))</f>
@@ -9624,23 +9747,23 @@
       </c>
       <c r="J10" s="8">
         <f>IF('ETS Coverage'!$B14=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B10)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B10)),IF('ETS Coverage'!$B14=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K10" s="8">
         <f>IF('ETS Coverage'!$B14=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B10)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B10)),IF('ETS Coverage'!$B14=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L10" s="8">
         <f>IF('ETS Coverage'!$B14=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B10)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B10)),IF('ETS Coverage'!$B14=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M10" s="8">
         <f>IF('ETS Coverage'!$B14=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B10)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B10)),IF('ETS Coverage'!$B14=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N10" s="8">
         <f>IF('ETS Coverage'!$B14=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B10)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B10)),IF('ETS Coverage'!$B14=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O10" s="8">
         <f>IF('ETS Coverage'!$B14=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B10)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B10)),IF('ETS Coverage'!$B14=2,'ETS Projections'!M$66,0))</f>
@@ -9771,79 +9894,79 @@
       </c>
       <c r="O11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!M$66,0))</f>
-        <v>0.71355731267957767</v>
+        <v>0.67796857964197832</v>
       </c>
       <c r="P11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!N$65*('Allowance Schedule'!P$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!P$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!N$66,0))</f>
-        <v>0.77054537138977963</v>
+        <v>0.70647446788667934</v>
       </c>
       <c r="Q11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!O$65*('Allowance Schedule'!Q$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!Q$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!O$66,0))</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="R11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!P$65*('Allowance Schedule'!R$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!R$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!P$66,0))</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="S11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!Q$65*('Allowance Schedule'!S$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!S$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!Q$66,0))</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="T11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!R$65*('Allowance Schedule'!T$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!T$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!R$66,0))</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="U11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!S$65*('Allowance Schedule'!U$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!U$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!S$66,0))</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="V11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!T$65*('Allowance Schedule'!V$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!V$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!T$66,0))</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="W11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!U$65*('Allowance Schedule'!W$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!W$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!U$66,0))</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="X11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!V$65*('Allowance Schedule'!X$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!X$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!V$66,0))</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="Y11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!W$65*('Allowance Schedule'!Y$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!Y$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!W$66,0))</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="Z11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!X$65*('Allowance Schedule'!Z$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!Z$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!X$66,0))</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="AA11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!Y$65*('Allowance Schedule'!AA$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!AA$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!Y$66,0))</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="AB11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!Z$65*('Allowance Schedule'!AB$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!AB$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!Z$66,0))</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AC11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!AA$65*('Allowance Schedule'!AC$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!AC$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!AA$66,0))</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AD11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!AB$65*('Allowance Schedule'!AD$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!AD$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!AB$66,0))</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AE11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!AC$65*('Allowance Schedule'!AE$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!AE$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!AC$66,0))</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AF11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!AD$65*('Allowance Schedule'!AF$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!AF$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!AD$66,0))</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AG11" s="8">
         <f>IF('ETS Coverage'!$B15=1,'ETS Projections'!AE$65*('Allowance Schedule'!AG$10*('Carbon Leakage Risk'!$B11)+'Allowance Schedule'!AG$11*(1-'Carbon Leakage Risk'!$B11)),IF('ETS Coverage'!$B15=2,'ETS Projections'!AE$66,0))</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="12" spans="1:33">
@@ -9898,79 +10021,79 @@
       </c>
       <c r="O12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!M$66,0))</f>
-        <v>0.71100954166939512</v>
+        <v>0.67554787893254264</v>
       </c>
       <c r="P12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!N$65*('Allowance Schedule'!P$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!P$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!N$66,0))</f>
-        <v>0.76930070734494993</v>
+        <v>0.70533329774742748</v>
       </c>
       <c r="Q12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!O$65*('Allowance Schedule'!Q$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!Q$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!O$66,0))</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="R12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!P$65*('Allowance Schedule'!R$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!R$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!P$66,0))</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="S12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!Q$65*('Allowance Schedule'!S$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!S$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!Q$66,0))</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="T12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!R$65*('Allowance Schedule'!T$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!T$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!R$66,0))</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="U12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!S$65*('Allowance Schedule'!U$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!U$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!S$66,0))</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="V12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!T$65*('Allowance Schedule'!V$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!V$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!T$66,0))</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="W12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!U$65*('Allowance Schedule'!W$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!W$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!U$66,0))</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="X12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!V$65*('Allowance Schedule'!X$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!X$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!V$66,0))</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="Y12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!W$65*('Allowance Schedule'!Y$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!Y$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!W$66,0))</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="Z12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!X$65*('Allowance Schedule'!Z$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!Z$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!X$66,0))</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="AA12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!Y$65*('Allowance Schedule'!AA$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!AA$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!Y$66,0))</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="AB12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!Z$65*('Allowance Schedule'!AB$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!AB$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!Z$66,0))</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AC12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!AA$65*('Allowance Schedule'!AC$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!AC$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!AA$66,0))</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AD12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!AB$65*('Allowance Schedule'!AD$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!AD$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!AB$66,0))</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AE12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!AC$65*('Allowance Schedule'!AE$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!AE$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!AC$66,0))</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AF12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!AD$65*('Allowance Schedule'!AF$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!AF$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!AD$66,0))</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AG12" s="8">
         <f>IF('ETS Coverage'!$B16=1,'ETS Projections'!AE$65*('Allowance Schedule'!AG$10*('Carbon Leakage Risk'!$B12)+'Allowance Schedule'!AG$11*(1-'Carbon Leakage Risk'!$B12)),IF('ETS Coverage'!$B16=2,'ETS Projections'!AE$66,0))</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="13" spans="1:33">
@@ -10025,79 +10148,79 @@
       </c>
       <c r="O13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!M$66,0))</f>
-        <v>0.736200028899056</v>
+        <v>0.69948198842046772</v>
       </c>
       <c r="P13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!N$65*('Allowance Schedule'!P$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!P$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!N$66,0))</f>
-        <v>0.78160703063742532</v>
+        <v>0.71661634936580532</v>
       </c>
       <c r="Q13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!O$65*('Allowance Schedule'!Q$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!Q$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!O$66,0))</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="R13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!P$65*('Allowance Schedule'!R$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!R$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!P$66,0))</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="S13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!Q$65*('Allowance Schedule'!S$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!S$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!Q$66,0))</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="T13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!R$65*('Allowance Schedule'!T$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!T$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!R$66,0))</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="U13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!S$65*('Allowance Schedule'!U$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!U$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!S$66,0))</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="V13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!T$65*('Allowance Schedule'!V$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!V$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!T$66,0))</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="W13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!U$65*('Allowance Schedule'!W$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!W$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!U$66,0))</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="X13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!V$65*('Allowance Schedule'!X$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!X$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!V$66,0))</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="Y13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!W$65*('Allowance Schedule'!Y$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!Y$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!W$66,0))</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="Z13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!X$65*('Allowance Schedule'!Z$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!Z$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!X$66,0))</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="AA13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!Y$65*('Allowance Schedule'!AA$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!AA$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!Y$66,0))</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="AB13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!Z$65*('Allowance Schedule'!AB$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!AB$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!Z$66,0))</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AC13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!AA$65*('Allowance Schedule'!AC$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!AC$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!AA$66,0))</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AD13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!AB$65*('Allowance Schedule'!AD$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!AD$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!AB$66,0))</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AE13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!AC$65*('Allowance Schedule'!AE$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!AE$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!AC$66,0))</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AF13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!AD$65*('Allowance Schedule'!AF$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!AF$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!AD$66,0))</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AG13" s="8">
         <f>IF('ETS Coverage'!$B17=1,'ETS Projections'!AE$65*('Allowance Schedule'!AG$10*('Carbon Leakage Risk'!$B13)+'Allowance Schedule'!AG$11*(1-'Carbon Leakage Risk'!$B13)),IF('ETS Coverage'!$B17=2,'ETS Projections'!AE$66,0))</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="14" spans="1:33">
@@ -10132,23 +10255,23 @@
       </c>
       <c r="J14" s="8">
         <f>IF('ETS Coverage'!$B18=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B14)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B14)),IF('ETS Coverage'!$B18=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K14" s="8">
         <f>IF('ETS Coverage'!$B18=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B14)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B14)),IF('ETS Coverage'!$B18=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L14" s="8">
         <f>IF('ETS Coverage'!$B18=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B14)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B14)),IF('ETS Coverage'!$B18=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M14" s="8">
         <f>IF('ETS Coverage'!$B18=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B14)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B14)),IF('ETS Coverage'!$B18=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N14" s="8">
         <f>IF('ETS Coverage'!$B18=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B14)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B14)),IF('ETS Coverage'!$B18=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O14" s="8">
         <f>IF('ETS Coverage'!$B18=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B14)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B14)),IF('ETS Coverage'!$B18=2,'ETS Projections'!M$66,0))</f>
@@ -10279,79 +10402,79 @@
       </c>
       <c r="O15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!M$66,0))</f>
-        <v>0.71100954166939512</v>
+        <v>0.67554787893254264</v>
       </c>
       <c r="P15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!N$65*('Allowance Schedule'!P$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!P$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!N$66,0))</f>
-        <v>0.76930070734494993</v>
+        <v>0.70533329774742748</v>
       </c>
       <c r="Q15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!O$65*('Allowance Schedule'!Q$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!Q$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!O$66,0))</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="R15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!P$65*('Allowance Schedule'!R$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!R$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!P$66,0))</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="S15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!Q$65*('Allowance Schedule'!S$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!S$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!Q$66,0))</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="T15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!R$65*('Allowance Schedule'!T$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!T$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!R$66,0))</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="U15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!S$65*('Allowance Schedule'!U$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!U$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!S$66,0))</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="V15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!T$65*('Allowance Schedule'!V$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!V$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!T$66,0))</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="W15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!U$65*('Allowance Schedule'!W$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!W$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!U$66,0))</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="X15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!V$65*('Allowance Schedule'!X$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!X$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!V$66,0))</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="Y15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!W$65*('Allowance Schedule'!Y$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!Y$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!W$66,0))</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="Z15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!X$65*('Allowance Schedule'!Z$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!Z$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!X$66,0))</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="AA15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!Y$65*('Allowance Schedule'!AA$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!AA$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!Y$66,0))</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="AB15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!Z$65*('Allowance Schedule'!AB$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!AB$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!Z$66,0))</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AC15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!AA$65*('Allowance Schedule'!AC$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!AC$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!AA$66,0))</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AD15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!AB$65*('Allowance Schedule'!AD$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!AD$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!AB$66,0))</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AE15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!AC$65*('Allowance Schedule'!AE$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!AE$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!AC$66,0))</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AF15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!AD$65*('Allowance Schedule'!AF$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!AF$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!AD$66,0))</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AG15" s="8">
         <f>IF('ETS Coverage'!$B19=1,'ETS Projections'!AE$65*('Allowance Schedule'!AG$10*('Carbon Leakage Risk'!$B15)+'Allowance Schedule'!AG$11*(1-'Carbon Leakage Risk'!$B15)),IF('ETS Coverage'!$B19=2,'ETS Projections'!AE$66,0))</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="16" spans="1:33">
@@ -10406,79 +10529,79 @@
       </c>
       <c r="O16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!M$66,0))</f>
-        <v>0.71100954166939512</v>
+        <v>0.67554787893254264</v>
       </c>
       <c r="P16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!N$65*('Allowance Schedule'!P$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!P$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!N$66,0))</f>
-        <v>0.76930070734494993</v>
+        <v>0.70533329774742748</v>
       </c>
       <c r="Q16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!O$65*('Allowance Schedule'!Q$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!Q$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!O$66,0))</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="R16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!P$65*('Allowance Schedule'!R$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!R$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!P$66,0))</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="S16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!Q$65*('Allowance Schedule'!S$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!S$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!Q$66,0))</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="T16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!R$65*('Allowance Schedule'!T$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!T$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!R$66,0))</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="U16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!S$65*('Allowance Schedule'!U$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!U$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!S$66,0))</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="V16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!T$65*('Allowance Schedule'!V$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!V$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!T$66,0))</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="W16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!U$65*('Allowance Schedule'!W$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!W$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!U$66,0))</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="X16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!V$65*('Allowance Schedule'!X$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!X$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!V$66,0))</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="Y16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!W$65*('Allowance Schedule'!Y$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!Y$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!W$66,0))</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="Z16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!X$65*('Allowance Schedule'!Z$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!Z$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!X$66,0))</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="AA16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!Y$65*('Allowance Schedule'!AA$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!AA$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!Y$66,0))</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="AB16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!Z$65*('Allowance Schedule'!AB$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!AB$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!Z$66,0))</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AC16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!AA$65*('Allowance Schedule'!AC$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!AC$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!AA$66,0))</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AD16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!AB$65*('Allowance Schedule'!AD$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!AD$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!AB$66,0))</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AE16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!AC$65*('Allowance Schedule'!AE$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!AE$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!AC$66,0))</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AF16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!AD$65*('Allowance Schedule'!AF$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!AF$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!AD$66,0))</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AG16" s="8">
         <f>IF('ETS Coverage'!$B20=1,'ETS Projections'!AE$65*('Allowance Schedule'!AG$10*('Carbon Leakage Risk'!$B16)+'Allowance Schedule'!AG$11*(1-'Carbon Leakage Risk'!$B16)),IF('ETS Coverage'!$B20=2,'ETS Projections'!AE$66,0))</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="17" spans="2:33">
@@ -10533,79 +10656,79 @@
       </c>
       <c r="O17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!M$66,0))</f>
-        <v>0.71100954166939512</v>
+        <v>0.67554787893254264</v>
       </c>
       <c r="P17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!N$65*('Allowance Schedule'!P$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!P$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!N$66,0))</f>
-        <v>0.76930070734494993</v>
+        <v>0.70533329774742748</v>
       </c>
       <c r="Q17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!O$65*('Allowance Schedule'!Q$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!Q$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!O$66,0))</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="R17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!P$65*('Allowance Schedule'!R$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!R$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!P$66,0))</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="S17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!Q$65*('Allowance Schedule'!S$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!S$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!Q$66,0))</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="T17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!R$65*('Allowance Schedule'!T$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!T$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!R$66,0))</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="U17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!S$65*('Allowance Schedule'!U$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!U$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!S$66,0))</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="V17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!T$65*('Allowance Schedule'!V$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!V$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!T$66,0))</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="W17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!U$65*('Allowance Schedule'!W$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!W$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!U$66,0))</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="X17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!V$65*('Allowance Schedule'!X$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!X$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!V$66,0))</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="Y17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!W$65*('Allowance Schedule'!Y$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!Y$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!W$66,0))</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="Z17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!X$65*('Allowance Schedule'!Z$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!Z$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!X$66,0))</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="AA17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!Y$65*('Allowance Schedule'!AA$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!AA$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!Y$66,0))</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="AB17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!Z$65*('Allowance Schedule'!AB$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!AB$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!Z$66,0))</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AC17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!AA$65*('Allowance Schedule'!AC$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!AC$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!AA$66,0))</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AD17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!AB$65*('Allowance Schedule'!AD$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!AD$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!AB$66,0))</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AE17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!AC$65*('Allowance Schedule'!AE$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!AE$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!AC$66,0))</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AF17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!AD$65*('Allowance Schedule'!AF$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!AF$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!AD$66,0))</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AG17" s="8">
         <f>IF('ETS Coverage'!$B21=1,'ETS Projections'!AE$65*('Allowance Schedule'!AG$10*('Carbon Leakage Risk'!$B17)+'Allowance Schedule'!AG$11*(1-'Carbon Leakage Risk'!$B17)),IF('ETS Coverage'!$B21=2,'ETS Projections'!AE$66,0))</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="18" spans="2:33">
@@ -10660,79 +10783,79 @@
       </c>
       <c r="O18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!M$66,0))</f>
-        <v>0.71100954166939512</v>
+        <v>0.67554787893254264</v>
       </c>
       <c r="P18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!N$65*('Allowance Schedule'!P$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!P$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!N$66,0))</f>
-        <v>0.76930070734494993</v>
+        <v>0.70533329774742748</v>
       </c>
       <c r="Q18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!O$65*('Allowance Schedule'!Q$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!Q$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!O$66,0))</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="R18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!P$65*('Allowance Schedule'!R$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!R$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!P$66,0))</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="S18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!Q$65*('Allowance Schedule'!S$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!S$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!Q$66,0))</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="T18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!R$65*('Allowance Schedule'!T$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!T$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!R$66,0))</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="U18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!S$65*('Allowance Schedule'!U$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!U$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!S$66,0))</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="V18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!T$65*('Allowance Schedule'!V$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!V$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!T$66,0))</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="W18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!U$65*('Allowance Schedule'!W$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!W$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!U$66,0))</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="X18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!V$65*('Allowance Schedule'!X$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!X$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!V$66,0))</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="Y18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!W$65*('Allowance Schedule'!Y$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!Y$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!W$66,0))</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="Z18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!X$65*('Allowance Schedule'!Z$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!Z$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!X$66,0))</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="AA18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!Y$65*('Allowance Schedule'!AA$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!AA$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!Y$66,0))</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="AB18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!Z$65*('Allowance Schedule'!AB$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!AB$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!Z$66,0))</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AC18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!AA$65*('Allowance Schedule'!AC$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!AC$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!AA$66,0))</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AD18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!AB$65*('Allowance Schedule'!AD$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!AD$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!AB$66,0))</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AE18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!AC$65*('Allowance Schedule'!AE$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!AE$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!AC$66,0))</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AF18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!AD$65*('Allowance Schedule'!AF$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!AF$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!AD$66,0))</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AG18" s="8">
         <f>IF('ETS Coverage'!$B22=1,'ETS Projections'!AE$65*('Allowance Schedule'!AG$10*('Carbon Leakage Risk'!$B18)+'Allowance Schedule'!AG$11*(1-'Carbon Leakage Risk'!$B18)),IF('ETS Coverage'!$B22=2,'ETS Projections'!AE$66,0))</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="19" spans="2:33">
@@ -10767,23 +10890,23 @@
       </c>
       <c r="J19" s="8">
         <f>IF('ETS Coverage'!$B23=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B19)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B19)),IF('ETS Coverage'!$B23=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K19" s="8">
         <f>IF('ETS Coverage'!$B23=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B19)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B19)),IF('ETS Coverage'!$B23=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L19" s="8">
         <f>IF('ETS Coverage'!$B23=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B19)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B19)),IF('ETS Coverage'!$B23=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M19" s="8">
         <f>IF('ETS Coverage'!$B23=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B19)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B19)),IF('ETS Coverage'!$B23=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N19" s="8">
         <f>IF('ETS Coverage'!$B23=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B19)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B19)),IF('ETS Coverage'!$B23=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O19" s="8">
         <f>IF('ETS Coverage'!$B23=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B19)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B19)),IF('ETS Coverage'!$B23=2,'ETS Projections'!M$66,0))</f>
@@ -10894,23 +11017,23 @@
       </c>
       <c r="J20" s="8">
         <f>IF('ETS Coverage'!$B24=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B20)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B20)),IF('ETS Coverage'!$B24=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K20" s="8">
         <f>IF('ETS Coverage'!$B24=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B20)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B20)),IF('ETS Coverage'!$B24=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L20" s="8">
         <f>IF('ETS Coverage'!$B24=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B20)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B20)),IF('ETS Coverage'!$B24=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M20" s="8">
         <f>IF('ETS Coverage'!$B24=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B20)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B20)),IF('ETS Coverage'!$B24=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N20" s="8">
         <f>IF('ETS Coverage'!$B24=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B20)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B20)),IF('ETS Coverage'!$B24=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O20" s="8">
         <f>IF('ETS Coverage'!$B24=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B20)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B20)),IF('ETS Coverage'!$B24=2,'ETS Projections'!M$66,0))</f>
@@ -11021,23 +11144,23 @@
       </c>
       <c r="J21" s="8">
         <f>IF('ETS Coverage'!$B25=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B21)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B21)),IF('ETS Coverage'!$B25=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K21" s="8">
         <f>IF('ETS Coverage'!$B25=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B21)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B21)),IF('ETS Coverage'!$B25=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L21" s="8">
         <f>IF('ETS Coverage'!$B25=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B21)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B21)),IF('ETS Coverage'!$B25=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M21" s="8">
         <f>IF('ETS Coverage'!$B25=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B21)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B21)),IF('ETS Coverage'!$B25=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N21" s="8">
         <f>IF('ETS Coverage'!$B25=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B21)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B21)),IF('ETS Coverage'!$B25=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O21" s="8">
         <f>IF('ETS Coverage'!$B25=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B21)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B21)),IF('ETS Coverage'!$B25=2,'ETS Projections'!M$66,0))</f>
@@ -11148,23 +11271,23 @@
       </c>
       <c r="J22" s="8">
         <f>IF('ETS Coverage'!$B26=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B22)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B22)),IF('ETS Coverage'!$B26=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K22" s="8">
         <f>IF('ETS Coverage'!$B26=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B22)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B22)),IF('ETS Coverage'!$B26=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L22" s="8">
         <f>IF('ETS Coverage'!$B26=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B22)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B22)),IF('ETS Coverage'!$B26=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M22" s="8">
         <f>IF('ETS Coverage'!$B26=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B22)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B22)),IF('ETS Coverage'!$B26=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N22" s="8">
         <f>IF('ETS Coverage'!$B26=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B22)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B22)),IF('ETS Coverage'!$B26=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O22" s="8">
         <f>IF('ETS Coverage'!$B26=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B22)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B22)),IF('ETS Coverage'!$B26=2,'ETS Projections'!M$66,0))</f>
@@ -11275,23 +11398,23 @@
       </c>
       <c r="J23" s="8">
         <f>IF('ETS Coverage'!$B27=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B23)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B23)),IF('ETS Coverage'!$B27=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K23" s="8">
         <f>IF('ETS Coverage'!$B27=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B23)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B23)),IF('ETS Coverage'!$B27=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L23" s="8">
         <f>IF('ETS Coverage'!$B27=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B23)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B23)),IF('ETS Coverage'!$B27=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M23" s="8">
         <f>IF('ETS Coverage'!$B27=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B23)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B23)),IF('ETS Coverage'!$B27=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N23" s="8">
         <f>IF('ETS Coverage'!$B27=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B23)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B23)),IF('ETS Coverage'!$B27=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O23" s="8">
         <f>IF('ETS Coverage'!$B27=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B23)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B23)),IF('ETS Coverage'!$B27=2,'ETS Projections'!M$66,0))</f>
@@ -11402,23 +11525,23 @@
       </c>
       <c r="J24" s="8">
         <f>IF('ETS Coverage'!$B28=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B24)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B24)),IF('ETS Coverage'!$B28=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K24" s="8">
         <f>IF('ETS Coverage'!$B28=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B24)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B24)),IF('ETS Coverage'!$B28=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L24" s="8">
         <f>IF('ETS Coverage'!$B28=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B24)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B24)),IF('ETS Coverage'!$B28=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M24" s="8">
         <f>IF('ETS Coverage'!$B28=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B24)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B24)),IF('ETS Coverage'!$B28=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N24" s="8">
         <f>IF('ETS Coverage'!$B28=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B24)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B24)),IF('ETS Coverage'!$B28=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O24" s="8">
         <f>IF('ETS Coverage'!$B28=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B24)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B24)),IF('ETS Coverage'!$B28=2,'ETS Projections'!M$66,0))</f>
@@ -11529,23 +11652,23 @@
       </c>
       <c r="J25" s="8">
         <f>IF('ETS Coverage'!$B29=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B25)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B25)),IF('ETS Coverage'!$B29=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K25" s="8">
         <f>IF('ETS Coverage'!$B29=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B25)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B25)),IF('ETS Coverage'!$B29=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L25" s="8">
         <f>IF('ETS Coverage'!$B29=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B25)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B25)),IF('ETS Coverage'!$B29=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M25" s="8">
         <f>IF('ETS Coverage'!$B29=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B25)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B25)),IF('ETS Coverage'!$B29=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N25" s="8">
         <f>IF('ETS Coverage'!$B29=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B25)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B25)),IF('ETS Coverage'!$B29=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O25" s="8">
         <f>IF('ETS Coverage'!$B29=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B25)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B25)),IF('ETS Coverage'!$B29=2,'ETS Projections'!M$66,0))</f>
@@ -11656,23 +11779,23 @@
       </c>
       <c r="J26" s="8">
         <f>IF('ETS Coverage'!$B30=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B26)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B26)),IF('ETS Coverage'!$B30=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K26" s="8">
         <f>IF('ETS Coverage'!$B30=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B26)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B26)),IF('ETS Coverage'!$B30=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L26" s="8">
         <f>IF('ETS Coverage'!$B30=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B26)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B26)),IF('ETS Coverage'!$B30=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M26" s="8">
         <f>IF('ETS Coverage'!$B30=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B26)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B26)),IF('ETS Coverage'!$B30=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N26" s="8">
         <f>IF('ETS Coverage'!$B30=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B26)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B26)),IF('ETS Coverage'!$B30=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O26" s="8">
         <f>IF('ETS Coverage'!$B30=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B26)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B26)),IF('ETS Coverage'!$B30=2,'ETS Projections'!M$66,0))</f>
@@ -11910,23 +12033,23 @@
       </c>
       <c r="J28" s="8">
         <f>IF('ETS Coverage'!$B32=1,'ETS Projections'!H$65*('Allowance Schedule'!J$10*('Carbon Leakage Risk'!$B28)+'Allowance Schedule'!J$11*(1-'Carbon Leakage Risk'!$B28)),IF('ETS Coverage'!$B32=2,'ETS Projections'!H$66,0))</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="K28" s="8">
         <f>IF('ETS Coverage'!$B32=1,'ETS Projections'!I$65*('Allowance Schedule'!K$10*('Carbon Leakage Risk'!$B28)+'Allowance Schedule'!K$11*(1-'Carbon Leakage Risk'!$B28)),IF('ETS Coverage'!$B32=2,'ETS Projections'!I$66,0))</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="L28" s="8">
         <f>IF('ETS Coverage'!$B32=1,'ETS Projections'!J$65*('Allowance Schedule'!L$10*('Carbon Leakage Risk'!$B28)+'Allowance Schedule'!L$11*(1-'Carbon Leakage Risk'!$B28)),IF('ETS Coverage'!$B32=2,'ETS Projections'!J$66,0))</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="M28" s="8">
         <f>IF('ETS Coverage'!$B32=1,'ETS Projections'!K$65*('Allowance Schedule'!M$10*('Carbon Leakage Risk'!$B28)+'Allowance Schedule'!M$11*(1-'Carbon Leakage Risk'!$B28)),IF('ETS Coverage'!$B32=2,'ETS Projections'!K$66,0))</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="N28" s="8">
         <f>IF('ETS Coverage'!$B32=1,'ETS Projections'!L$65*('Allowance Schedule'!N$10*('Carbon Leakage Risk'!$B28)+'Allowance Schedule'!N$11*(1-'Carbon Leakage Risk'!$B28)),IF('ETS Coverage'!$B32=2,'ETS Projections'!L$66,0))</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="O28" s="8">
         <f>IF('ETS Coverage'!$B32=1,'ETS Projections'!M$65*('Allowance Schedule'!O$10*('Carbon Leakage Risk'!$B28)+'Allowance Schedule'!O$11*(1-'Carbon Leakage Risk'!$B28)),IF('ETS Coverage'!$B32=2,'ETS Projections'!M$66,0))</f>
@@ -12027,10 +12150,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AE28"/>
+  <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="B27" sqref="A27:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -12289,23 +12412,23 @@
       </c>
       <c r="H3" s="7">
         <f>Calcs!J5</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I3" s="7">
         <f>Calcs!K5</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J3" s="7">
         <f>Calcs!L5</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K3" s="7">
         <f>Calcs!M5</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L3" s="7">
         <f>Calcs!N5</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M3" s="7">
         <f>Calcs!O5</f>
@@ -12414,23 +12537,23 @@
       </c>
       <c r="H4" s="7">
         <f>Calcs!J6</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I4" s="7">
         <f>Calcs!K6</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J4" s="7">
         <f>Calcs!L6</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K4" s="7">
         <f>Calcs!M6</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L4" s="7">
         <f>Calcs!N6</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M4" s="7">
         <f>Calcs!O6</f>
@@ -12539,23 +12662,23 @@
       </c>
       <c r="H5" s="7">
         <f>Calcs!J7</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I5" s="7">
         <f>Calcs!K7</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J5" s="7">
         <f>Calcs!L7</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K5" s="7">
         <f>Calcs!M7</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L5" s="7">
         <f>Calcs!N7</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M5" s="7">
         <f>Calcs!O7</f>
@@ -12664,23 +12787,23 @@
       </c>
       <c r="H6" s="7">
         <f>Calcs!J8</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I6" s="7">
         <f>Calcs!K8</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J6" s="7">
         <f>Calcs!L8</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K6" s="7">
         <f>Calcs!M8</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L6" s="7">
         <f>Calcs!N8</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M6" s="7">
         <f>Calcs!O8</f>
@@ -12789,23 +12912,23 @@
       </c>
       <c r="H7" s="7">
         <f>Calcs!J9</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I7" s="7">
         <f>Calcs!K9</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J7" s="7">
         <f>Calcs!L9</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K7" s="7">
         <f>Calcs!M9</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L7" s="7">
         <f>Calcs!N9</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M7" s="7">
         <f>Calcs!O9</f>
@@ -12914,23 +13037,23 @@
       </c>
       <c r="H8" s="7">
         <f>Calcs!J10</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I8" s="7">
         <f>Calcs!K10</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J8" s="7">
         <f>Calcs!L10</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K8" s="7">
         <f>Calcs!M10</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L8" s="7">
         <f>Calcs!N10</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M8" s="7">
         <f>Calcs!O10</f>
@@ -13059,79 +13182,79 @@
       </c>
       <c r="M9" s="7">
         <f>Calcs!O11</f>
-        <v>0.71355731267957767</v>
+        <v>0.67796857964197832</v>
       </c>
       <c r="N9" s="7">
         <f>Calcs!P11</f>
-        <v>0.77054537138977963</v>
+        <v>0.70647446788667934</v>
       </c>
       <c r="O9" s="7">
         <f>Calcs!Q11</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="P9" s="7">
         <f>Calcs!R11</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="Q9" s="7">
         <f>Calcs!S11</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="R9" s="7">
         <f>Calcs!T11</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="S9" s="7">
         <f>Calcs!U11</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="T9" s="7">
         <f>Calcs!V11</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="U9" s="7">
         <f>Calcs!W11</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="V9" s="7">
         <f>Calcs!X11</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="W9" s="7">
         <f>Calcs!Y11</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="X9" s="7">
         <f>Calcs!Z11</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="Y9" s="7">
         <f>Calcs!AA11</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="Z9" s="7">
         <f>Calcs!AB11</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AA9" s="7">
         <f>Calcs!AC11</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AB9" s="7">
         <f>Calcs!AD11</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AC9" s="7">
         <f>Calcs!AE11</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AD9" s="7">
         <f>Calcs!AF11</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AE9" s="7">
         <f>Calcs!AG11</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -13184,79 +13307,79 @@
       </c>
       <c r="M10" s="7">
         <f>Calcs!O12</f>
-        <v>0.71100954166939512</v>
+        <v>0.67554787893254264</v>
       </c>
       <c r="N10" s="7">
         <f>Calcs!P12</f>
-        <v>0.76930070734494993</v>
+        <v>0.70533329774742748</v>
       </c>
       <c r="O10" s="7">
         <f>Calcs!Q12</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="P10" s="7">
         <f>Calcs!R12</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="Q10" s="7">
         <f>Calcs!S12</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="R10" s="7">
         <f>Calcs!T12</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="S10" s="7">
         <f>Calcs!U12</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="T10" s="7">
         <f>Calcs!V12</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="U10" s="7">
         <f>Calcs!W12</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="V10" s="7">
         <f>Calcs!X12</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="W10" s="7">
         <f>Calcs!Y12</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="X10" s="7">
         <f>Calcs!Z12</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="Y10" s="7">
         <f>Calcs!AA12</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="Z10" s="7">
         <f>Calcs!AB12</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AA10" s="7">
         <f>Calcs!AC12</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AB10" s="7">
         <f>Calcs!AD12</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AC10" s="7">
         <f>Calcs!AE12</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AD10" s="7">
         <f>Calcs!AF12</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AE10" s="7">
         <f>Calcs!AG12</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="11" spans="1:31">
@@ -13309,79 +13432,79 @@
       </c>
       <c r="M11" s="7">
         <f>Calcs!O13</f>
-        <v>0.736200028899056</v>
+        <v>0.69948198842046772</v>
       </c>
       <c r="N11" s="7">
         <f>Calcs!P13</f>
-        <v>0.78160703063742532</v>
+        <v>0.71661634936580532</v>
       </c>
       <c r="O11" s="7">
         <f>Calcs!Q13</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="P11" s="7">
         <f>Calcs!R13</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="Q11" s="7">
         <f>Calcs!S13</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="R11" s="7">
         <f>Calcs!T13</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="S11" s="7">
         <f>Calcs!U13</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="T11" s="7">
         <f>Calcs!V13</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="U11" s="7">
         <f>Calcs!W13</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="V11" s="7">
         <f>Calcs!X13</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="W11" s="7">
         <f>Calcs!Y13</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="X11" s="7">
         <f>Calcs!Z13</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="Y11" s="7">
         <f>Calcs!AA13</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="Z11" s="7">
         <f>Calcs!AB13</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AA11" s="7">
         <f>Calcs!AC13</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AB11" s="7">
         <f>Calcs!AD13</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AC11" s="7">
         <f>Calcs!AE13</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AD11" s="7">
         <f>Calcs!AF13</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AE11" s="7">
         <f>Calcs!AG13</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="12" spans="1:31">
@@ -13414,23 +13537,23 @@
       </c>
       <c r="H12" s="7">
         <f>Calcs!J14</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I12" s="7">
         <f>Calcs!K14</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J12" s="7">
         <f>Calcs!L14</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K12" s="7">
         <f>Calcs!M14</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L12" s="7">
         <f>Calcs!N14</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M12" s="7">
         <f>Calcs!O14</f>
@@ -13559,79 +13682,79 @@
       </c>
       <c r="M13" s="7">
         <f>Calcs!O15</f>
-        <v>0.71100954166939512</v>
+        <v>0.67554787893254264</v>
       </c>
       <c r="N13" s="7">
         <f>Calcs!P15</f>
-        <v>0.76930070734494993</v>
+        <v>0.70533329774742748</v>
       </c>
       <c r="O13" s="7">
         <f>Calcs!Q15</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="P13" s="7">
         <f>Calcs!R15</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="Q13" s="7">
         <f>Calcs!S15</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="R13" s="7">
         <f>Calcs!T15</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="S13" s="7">
         <f>Calcs!U15</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="T13" s="7">
         <f>Calcs!V15</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="U13" s="7">
         <f>Calcs!W15</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="V13" s="7">
         <f>Calcs!X15</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="W13" s="7">
         <f>Calcs!Y15</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="X13" s="7">
         <f>Calcs!Z15</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="Y13" s="7">
         <f>Calcs!AA15</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="Z13" s="7">
         <f>Calcs!AB15</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AA13" s="7">
         <f>Calcs!AC15</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AB13" s="7">
         <f>Calcs!AD15</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AC13" s="7">
         <f>Calcs!AE15</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AD13" s="7">
         <f>Calcs!AF15</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AE13" s="7">
         <f>Calcs!AG15</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="14" spans="1:31">
@@ -13684,79 +13807,79 @@
       </c>
       <c r="M14" s="7">
         <f>Calcs!O16</f>
-        <v>0.71100954166939512</v>
+        <v>0.67554787893254264</v>
       </c>
       <c r="N14" s="7">
         <f>Calcs!P16</f>
-        <v>0.76930070734494993</v>
+        <v>0.70533329774742748</v>
       </c>
       <c r="O14" s="7">
         <f>Calcs!Q16</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="P14" s="7">
         <f>Calcs!R16</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="Q14" s="7">
         <f>Calcs!S16</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="R14" s="7">
         <f>Calcs!T16</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="S14" s="7">
         <f>Calcs!U16</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="T14" s="7">
         <f>Calcs!V16</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="U14" s="7">
         <f>Calcs!W16</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="V14" s="7">
         <f>Calcs!X16</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="W14" s="7">
         <f>Calcs!Y16</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="X14" s="7">
         <f>Calcs!Z16</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="Y14" s="7">
         <f>Calcs!AA16</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="Z14" s="7">
         <f>Calcs!AB16</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AA14" s="7">
         <f>Calcs!AC16</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AB14" s="7">
         <f>Calcs!AD16</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AC14" s="7">
         <f>Calcs!AE16</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AD14" s="7">
         <f>Calcs!AF16</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AE14" s="7">
         <f>Calcs!AG16</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -13809,79 +13932,79 @@
       </c>
       <c r="M15" s="7">
         <f>Calcs!O17</f>
-        <v>0.71100954166939512</v>
+        <v>0.67554787893254264</v>
       </c>
       <c r="N15" s="7">
         <f>Calcs!P17</f>
-        <v>0.76930070734494993</v>
+        <v>0.70533329774742748</v>
       </c>
       <c r="O15" s="7">
         <f>Calcs!Q17</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="P15" s="7">
         <f>Calcs!R17</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="Q15" s="7">
         <f>Calcs!S17</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="R15" s="7">
         <f>Calcs!T17</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="S15" s="7">
         <f>Calcs!U17</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="T15" s="7">
         <f>Calcs!V17</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="U15" s="7">
         <f>Calcs!W17</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="V15" s="7">
         <f>Calcs!X17</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="W15" s="7">
         <f>Calcs!Y17</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="X15" s="7">
         <f>Calcs!Z17</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="Y15" s="7">
         <f>Calcs!AA17</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="Z15" s="7">
         <f>Calcs!AB17</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AA15" s="7">
         <f>Calcs!AC17</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AB15" s="7">
         <f>Calcs!AD17</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AC15" s="7">
         <f>Calcs!AE17</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AD15" s="7">
         <f>Calcs!AF17</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AE15" s="7">
         <f>Calcs!AG17</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="16" spans="1:31">
@@ -13934,79 +14057,79 @@
       </c>
       <c r="M16" s="7">
         <f>Calcs!O18</f>
-        <v>0.71100954166939512</v>
+        <v>0.67554787893254264</v>
       </c>
       <c r="N16" s="7">
         <f>Calcs!P18</f>
-        <v>0.76930070734494993</v>
+        <v>0.70533329774742748</v>
       </c>
       <c r="O16" s="7">
         <f>Calcs!Q18</f>
-        <v>0.83838180663913453</v>
+        <v>0.76702920449344913</v>
       </c>
       <c r="P16" s="7">
         <f>Calcs!R18</f>
-        <v>0.78985203256864778</v>
+        <v>0.71887152156448098</v>
       </c>
       <c r="Q16" s="7">
         <f>Calcs!S18</f>
-        <v>0.75791500330060757</v>
+        <v>0.68980453195441105</v>
       </c>
       <c r="R16" s="7">
         <f>Calcs!T18</f>
-        <v>0.73136368603754465</v>
+        <v>0.66563926421639297</v>
       </c>
       <c r="S16" s="7">
         <f>Calcs!U18</f>
-        <v>0.70999235157120133</v>
+        <v>0.64618847711678717</v>
       </c>
       <c r="T16" s="7">
         <f>Calcs!V18</f>
-        <v>0.69271912973048044</v>
+        <v>0.6304675233748841</v>
       </c>
       <c r="U16" s="7">
         <f>Calcs!W18</f>
-        <v>0.67875131944211387</v>
+        <v>0.61775493845911467</v>
       </c>
       <c r="V16" s="7">
         <f>Calcs!X18</f>
-        <v>0.68461029608502533</v>
+        <v>0.62308739476792896</v>
       </c>
       <c r="W16" s="7">
         <f>Calcs!Y18</f>
-        <v>0.69101512169112456</v>
+        <v>0.62891664700627326</v>
       </c>
       <c r="X16" s="7">
         <f>Calcs!Z18</f>
-        <v>0.697933233911742</v>
+        <v>0.63521305905982683</v>
       </c>
       <c r="Y16" s="7">
         <f>Calcs!AA18</f>
-        <v>0.70533719795302263</v>
+        <v>0.641951661578396</v>
       </c>
       <c r="Z16" s="7">
         <f>Calcs!AB18</f>
-        <v>0.71409093639190402</v>
+        <v>0.64991874023548524</v>
       </c>
       <c r="AA16" s="7">
         <f>Calcs!AC18</f>
-        <v>0.7382660168949674</v>
+        <v>0.6719213131081081</v>
       </c>
       <c r="AB16" s="7">
         <f>Calcs!AD18</f>
-        <v>0.76290309191727668</v>
+        <v>0.69434436309455783</v>
       </c>
       <c r="AC16" s="7">
         <f>Calcs!AE18</f>
-        <v>0.78801380181806213</v>
+        <v>0.71719848448643142</v>
       </c>
       <c r="AD16" s="7">
         <f>Calcs!AF18</f>
-        <v>0.81360995545207615</v>
+        <v>0.74049442492889994</v>
       </c>
       <c r="AE16" s="7">
         <f>Calcs!AG18</f>
-        <v>0.83970353718125812</v>
+        <v>0.76424309180226624</v>
       </c>
     </row>
     <row r="17" spans="1:31">
@@ -14039,23 +14162,23 @@
       </c>
       <c r="H17" s="7">
         <f>Calcs!J19</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I17" s="7">
         <f>Calcs!K19</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J17" s="7">
         <f>Calcs!L19</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K17" s="7">
         <f>Calcs!M19</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L17" s="7">
         <f>Calcs!N19</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M17" s="7">
         <f>Calcs!O19</f>
@@ -14164,23 +14287,23 @@
       </c>
       <c r="H18" s="7">
         <f>Calcs!J20</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I18" s="7">
         <f>Calcs!K20</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J18" s="7">
         <f>Calcs!L20</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K18" s="7">
         <f>Calcs!M20</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L18" s="7">
         <f>Calcs!N20</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M18" s="7">
         <f>Calcs!O20</f>
@@ -14289,23 +14412,23 @@
       </c>
       <c r="H19" s="7">
         <f>Calcs!J21</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I19" s="7">
         <f>Calcs!K21</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J19" s="7">
         <f>Calcs!L21</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K19" s="7">
         <f>Calcs!M21</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L19" s="7">
         <f>Calcs!N21</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M19" s="7">
         <f>Calcs!O21</f>
@@ -14414,23 +14537,23 @@
       </c>
       <c r="H20" s="7">
         <f>Calcs!J22</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I20" s="7">
         <f>Calcs!K22</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J20" s="7">
         <f>Calcs!L22</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K20" s="7">
         <f>Calcs!M22</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L20" s="7">
         <f>Calcs!N22</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M20" s="7">
         <f>Calcs!O22</f>
@@ -14539,23 +14662,23 @@
       </c>
       <c r="H21" s="7">
         <f>Calcs!J23</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I21" s="7">
         <f>Calcs!K23</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J21" s="7">
         <f>Calcs!L23</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K21" s="7">
         <f>Calcs!M23</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L21" s="7">
         <f>Calcs!N23</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M21" s="7">
         <f>Calcs!O23</f>
@@ -14664,23 +14787,23 @@
       </c>
       <c r="H22" s="7">
         <f>Calcs!J24</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I22" s="7">
         <f>Calcs!K24</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J22" s="7">
         <f>Calcs!L24</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K22" s="7">
         <f>Calcs!M24</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L22" s="7">
         <f>Calcs!N24</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M22" s="7">
         <f>Calcs!O24</f>
@@ -14789,23 +14912,23 @@
       </c>
       <c r="H23" s="7">
         <f>Calcs!J25</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I23" s="7">
         <f>Calcs!K25</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J23" s="7">
         <f>Calcs!L25</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K23" s="7">
         <f>Calcs!M25</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L23" s="7">
         <f>Calcs!N25</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M23" s="7">
         <f>Calcs!O25</f>
@@ -14914,23 +15037,23 @@
       </c>
       <c r="H24" s="7">
         <f>Calcs!J26</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I24" s="7">
         <f>Calcs!K26</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J24" s="7">
         <f>Calcs!L26</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K24" s="7">
         <f>Calcs!M26</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L24" s="7">
         <f>Calcs!N26</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M24" s="7">
         <f>Calcs!O26</f>
@@ -15164,23 +15287,23 @@
       </c>
       <c r="H26" s="7">
         <f>Calcs!J28</f>
-        <v>0.48235390993499733</v>
+        <v>0.4825395020511708</v>
       </c>
       <c r="I26" s="7">
         <f>Calcs!K28</f>
-        <v>0.67685018626478843</v>
+        <v>0.66393045842516363</v>
       </c>
       <c r="J26" s="7">
         <f>Calcs!L28</f>
-        <v>0.78728801286744277</v>
+        <v>0.77077996942773064</v>
       </c>
       <c r="K26" s="7">
         <f>Calcs!M28</f>
-        <v>0.85416264100303552</v>
+        <v>0.85792340111752319</v>
       </c>
       <c r="L26" s="7">
         <f>Calcs!N28</f>
-        <v>0.93297166200719062</v>
+        <v>0.95998088009684113</v>
       </c>
       <c r="M26" s="7">
         <f>Calcs!O28</f>
@@ -15258,10 +15381,6 @@
         <f>Calcs!AG28</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:31">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>